<commit_message>
Working as Downloadble w/files
</commit_message>
<xml_diff>
--- a/LabSignup/LabSignup/bin/Debug/ExcelFiles/SignInSheet.xlsx
+++ b/LabSignup/LabSignup/bin/Debug/ExcelFiles/SignInSheet.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CODING\LabSignup\LabSignup\LabSignup\bin\Debug\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CA2DC5-BBA9-4CC6-BD05-EF04D039FD09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0932DB-A7A7-4860-BE02-3CEB1A0D684B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="2640" windowWidth="21600" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32310" yWindow="4050" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>FirstName</t>
   </si>
@@ -52,44 +52,22 @@
   </si>
   <si>
     <t>LabHours</t>
-  </si>
-  <si>
-    <t>Justin</t>
-  </si>
-  <si>
-    <t>Keating</t>
-  </si>
-  <si>
-    <t>RN</t>
-  </si>
-  <si>
-    <t>4/24/2023 - What are STD's</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4/24/2023 </t>
-  </si>
-  <si>
-    <t>4:00PM</t>
-  </si>
-  <si>
-    <t>6:00PM</t>
-  </si>
-  <si>
-    <t>4/24/2023 12:48:20 AM</t>
-  </si>
-  <si>
-    <t>02:00:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -397,83 +375,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD22"/>
+      <selection activeCell="A2" sqref="A2:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="1" width="10.140625" customWidth="1"/>
-    <col min="2" max="2" bestFit="1" width="9.7109375" customWidth="1"/>
-    <col min="4" max="4" bestFit="1" width="26.42578125" customWidth="1"/>
-    <col min="5" max="5" bestFit="1" width="10.140625" customWidth="1"/>
-    <col min="6" max="6" bestFit="1" width="8.140625" customWidth="1"/>
-    <col min="7" max="7" bestFit="1" width="7.42578125" customWidth="1"/>
-    <col min="8" max="8" bestFit="1" width="19.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Working with version 1.05
</commit_message>
<xml_diff>
--- a/LabSignup/LabSignup/bin/Debug/ExcelFiles/SignInSheet.xlsx
+++ b/LabSignup/LabSignup/bin/Debug/ExcelFiles/SignInSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CODING\LabSignup\LabSignup\LabSignup\bin\Debug\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0932DB-A7A7-4860-BE02-3CEB1A0D684B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8CB7A6-5570-4ABA-9327-EA36E9F9333A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32310" yWindow="4050" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31470" yWindow="3525" windowWidth="18900" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,16 +58,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -378,7 +372,7 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD13"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,7 +416,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>